<commit_message>
Add 13 test cases for ATT prepaid page.
</commit_message>
<xml_diff>
--- a/com.att/src/test/resources/TestData.xlsx
+++ b/com.att/src/test/resources/TestData.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.att/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96516656-7E86-3347-8BD8-A96270D9C8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="Expedia" sheetId="1" r:id="rId1"/>
     <sheet name="Ebay" sheetId="2" r:id="rId2"/>
     <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
-    <sheet name="ATT" sheetId="4" r:id="rId4"/>
-    <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
-    <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
-    <sheet name="Trulia" sheetId="7" r:id="rId7"/>
-    <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
-    <sheet name="OverStock" sheetId="9" r:id="rId9"/>
-    <sheet name="ESPN" sheetId="10" r:id="rId10"/>
-    <sheet name="Verizon" sheetId="11" r:id="rId11"/>
-    <sheet name="Chase" sheetId="12" r:id="rId12"/>
-    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId13"/>
-    <sheet name="Redfin" sheetId="14" r:id="rId14"/>
+    <sheet name="ATT_LoginData" sheetId="15" r:id="rId4"/>
+    <sheet name="ATT" sheetId="4" r:id="rId5"/>
+    <sheet name="BankOfAmerica" sheetId="5" r:id="rId6"/>
+    <sheet name="BMWUSA" sheetId="6" r:id="rId7"/>
+    <sheet name="Trulia" sheetId="7" r:id="rId8"/>
+    <sheet name="AirBNB" sheetId="8" r:id="rId9"/>
+    <sheet name="OverStock" sheetId="9" r:id="rId10"/>
+    <sheet name="ESPN" sheetId="10" r:id="rId11"/>
+    <sheet name="Verizon" sheetId="11" r:id="rId12"/>
+    <sheet name="Chase" sheetId="12" r:id="rId13"/>
+    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId14"/>
+    <sheet name="Redfin" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,22 +48,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>https://www.att.com/prepaid/plans/</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>https://www.att.com/buy/prepaid-phones/</t>
+  </si>
+  <si>
+    <t>https://www.att.com/buy/wireless/prepaid/devices</t>
+  </si>
+  <si>
+    <t>https://www.paygonline.com/websc/loginPage.html</t>
+  </si>
+  <si>
+    <t>https://www.att.com/prepaid/deals/</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>asdfghqwer</t>
+  </si>
+  <si>
+    <t>9815672312</t>
+  </si>
+  <si>
+    <t>8454730402</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Andale Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,8 +125,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,15 +449,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -419,13 +477,13 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -433,13 +491,13 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A4ED8F-84C7-4351-B184-022F160E827E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -447,13 +505,13 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1F144-5BE0-43B5-8C2F-943F03339C79}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -461,13 +519,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C25186B-8AE5-4703-8BDB-6D9F1A2F53C3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -475,7 +533,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +547,7 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,27 +561,112 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81217741-8520-0246-B040-6E36329E2175}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB124C4-9CEE-457F-95C0-47C63DA908AF}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -531,9 +674,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -551,43 +694,31 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test cases to com.att
</commit_message>
<xml_diff>
--- a/com.att/src/test/resources/TestData.xlsx
+++ b/com.att/src/test/resources/TestData.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\com.att\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5254AACC-AD9E-44E8-85A4-D1A147A17C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
-    <sheet name="Expedia" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
-    <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
-    <sheet name="ATT" sheetId="4" r:id="rId4"/>
-    <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
-    <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
-    <sheet name="Trulia" sheetId="7" r:id="rId7"/>
-    <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
-    <sheet name="OverStock" sheetId="9" r:id="rId9"/>
-    <sheet name="ESPN" sheetId="10" r:id="rId10"/>
-    <sheet name="Verizon" sheetId="11" r:id="rId11"/>
-    <sheet name="Chase" sheetId="12" r:id="rId12"/>
-    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId13"/>
-    <sheet name="Redfin" sheetId="14" r:id="rId14"/>
+    <sheet name="TopLeftMenu" sheetId="15" r:id="rId1"/>
+    <sheet name="TopCenterMenu" sheetId="17" r:id="rId2"/>
+    <sheet name="TopHamburgerMenu" sheetId="18" r:id="rId3"/>
+    <sheet name="PhoneMenuBar" sheetId="19" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,17 +37,112 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>A</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+  <si>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>Wireless</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Prepaid</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Center Menu</t>
+  </si>
+  <si>
+    <t>Explore wireless</t>
+  </si>
+  <si>
+    <t>Plans &amp; prices</t>
+  </si>
+  <si>
+    <t>Phones &amp; devices</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>Bring your own</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Wireless deals</t>
+  </si>
+  <si>
+    <t>Left Menu</t>
+  </si>
+  <si>
+    <t>Deals &amp; discounts</t>
+  </si>
+  <si>
+    <t>Home phone</t>
+  </si>
+  <si>
+    <t>Bundles</t>
+  </si>
+  <si>
+    <t>Smart technology</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Find a store</t>
+  </si>
+  <si>
+    <t>Check order status</t>
+  </si>
+  <si>
+    <t>My favorites</t>
+  </si>
+  <si>
+    <t>Hamburger Menu</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>AT&amp;T PREPAID</t>
+  </si>
+  <si>
+    <t>Tablets &amp; Laptops</t>
+  </si>
+  <si>
+    <t>Smartwatches</t>
+  </si>
+  <si>
+    <t>Hotspots &amp; more</t>
+  </si>
+  <si>
+    <t>Phone Menu Bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,8 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,195 +486,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E464D8A-6350-4BC5-B9EB-BA5543395498}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A4ED8F-84C7-4351-B184-022F160E827E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1F144-5BE0-43B5-8C2F-943F03339C79}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C25186B-8AE5-4703-8BDB-6D9F1A2F53C3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA0B8EC-E04F-491E-87C2-487F73A9BC0A}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59BB938-FA52-426E-9DD7-96F933A4DBB1}">
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CA77FC-C852-40C4-B844-304E3F0A9E58}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB124C4-9CEE-457F-95C0-47C63DA908AF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
complete some test cases on ESPN,ATT,BOA,Expedia
</commit_message>
<xml_diff>
--- a/com.att/src/test/resources/TestData.xlsx
+++ b/com.att/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khadizapushpo/IdeaProjects/Team1BootCamp/com.att/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AAD098-5D99-C143-BCE4-749B0994FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="20" yWindow="1280" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="Expedia" sheetId="1" r:id="rId1"/>
@@ -47,22 +47,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>AT&amp;T Official Site - Unlimited Data Plans, Internet Service, &amp; TV</t>
+  </si>
+  <si>
+    <t>Att:Accessories</t>
+  </si>
+  <si>
+    <t>Att:Headphones</t>
+  </si>
+  <si>
+    <t>Att:Cases</t>
+  </si>
+  <si>
+    <t>Att:Chargers</t>
+  </si>
+  <si>
+    <t>Att:Screen Protectors</t>
+  </si>
+  <si>
+    <t>Att:Speakers And Smart Home</t>
+  </si>
+  <si>
+    <t>Att:Internet And Tv Equipment</t>
+  </si>
+  <si>
+    <t>Att:Pop Sockets And More</t>
+  </si>
+  <si>
+    <t>Att:Gadgets And Gaming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF008000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,13 +130,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,9 +456,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -419,7 +472,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -433,7 +486,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -447,7 +500,7 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,7 +514,7 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,7 +528,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +542,7 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,7 +556,7 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -511,15 +564,76 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="53.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -531,9 +645,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +665,7 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -563,7 +677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -575,7 +689,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -587,7 +701,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some testcases in ATT And CBSSPORTS
</commit_message>
<xml_diff>
--- a/com.att/src/test/resources/TestData.xlsx
+++ b/com.att/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khadizapushpo/IdeaProjects/Team1BootCamp/com.att/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AAD098-5D99-C143-BCE4-749B0994FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E178FB-36B2-A849-B445-9E2FEEB7EB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1280" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="7280" yWindow="1440" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="Expedia" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -55,52 +55,71 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>AT&amp;T Official Site - Unlimited Data Plans, Internet Service, &amp; TV</t>
-  </si>
-  <si>
-    <t>Att:Accessories</t>
-  </si>
-  <si>
-    <t>Att:Headphones</t>
-  </si>
-  <si>
-    <t>Att:Cases</t>
-  </si>
-  <si>
-    <t>Att:Chargers</t>
-  </si>
-  <si>
-    <t>Att:Screen Protectors</t>
-  </si>
-  <si>
-    <t>Att:Speakers And Smart Home</t>
-  </si>
-  <si>
-    <t>Att:Internet And Tv Equipment</t>
-  </si>
-  <si>
-    <t>Att:Pop Sockets And More</t>
-  </si>
-  <si>
-    <t>Att:Gadgets And Gaming</t>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>Wireless</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Prepaid</t>
+  </si>
+  <si>
+    <t>Bundles</t>
+  </si>
+  <si>
+    <t>My Favourite icon</t>
+  </si>
+  <si>
+    <t>Cart icon</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Account Drop Down Menu</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>Create one Now</t>
+  </si>
+  <si>
+    <t>Home phone</t>
+  </si>
+  <si>
+    <t>Phones &amp; devices</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>HamBurger menu Icon</t>
+  </si>
+  <si>
+    <t>Accessories Deals</t>
+  </si>
+  <si>
+    <t>Account Number And Zip Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,18 +149,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -564,10 +580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -586,49 +602,94 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>